<commit_message>
BOM finished and Gerber files created
</commit_message>
<xml_diff>
--- a/hardware/PCB/BOM_v0.1_r1.xlsx
+++ b/hardware/PCB/BOM_v0.1_r1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meier\Documents\Repos\lora\hardware\PCB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41C4A60A-3F81-4419-9F9A-76F85301C1FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58D480D3-5B87-478B-87A9-539D5A529EE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16896" xr2:uid="{BC3F5926-5C61-49F0-80BB-A13677373133}"/>
+    <workbookView xWindow="16332" yWindow="720" windowWidth="25644" windowHeight="15960" xr2:uid="{BC3F5926-5C61-49F0-80BB-A13677373133}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="77">
   <si>
     <t>Id</t>
   </si>
@@ -102,24 +102,12 @@
     <t>SW_SPST</t>
   </si>
   <si>
-    <t>J3</t>
-  </si>
-  <si>
-    <t>Battery connector</t>
-  </si>
-  <si>
     <t>J2</t>
   </si>
   <si>
     <t>Power layer connector</t>
   </si>
   <si>
-    <t>J4</t>
-  </si>
-  <si>
-    <t>PinSocket_1x04_P2.54mm_Vertical</t>
-  </si>
-  <si>
     <t>AM2320</t>
   </si>
   <si>
@@ -216,9 +204,6 @@
     <t>https://www.mouser.ch/ProductDetail/YAGEO/RT1206FRE07330RL?qs=sGAEpiMZZMtlubZbdhIBIIe0KCL5sPzhE2j83oVm%252Bew%3D</t>
   </si>
   <si>
-    <t>X</t>
-  </si>
-  <si>
     <t>https://www.mouser.ch/ProductDetail/Keystone-Electronics/3000?qs=sGAEpiMZZMvxX9Q80wbhCYuFHF%2FXyzv7</t>
   </si>
   <si>
@@ -255,13 +240,31 @@
     <t>https://www.seeedstudio.com/Grove-Universal-4-pin-connector.html</t>
   </si>
   <si>
-    <t>distrelec</t>
-  </si>
-  <si>
-    <t>distrelec??</t>
-  </si>
-  <si>
     <t>JLCPCB</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ch/ProductDetail/Harwin/M20-7820242?qs=WS5Jv%252B%252Bx1qUrSLY%252BudG7mQ%3D%3D</t>
+  </si>
+  <si>
+    <t>PinSocket_1x14_P2.54mm_Vertical</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ch/ProductDetail/Harwin/M20-7821446?qs=Jph8NoUxIfX%2FjYzLF0Toqw%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ch/ProductDetail/Samtec/TSW-102-17-L-S?qs=rU5fayqh%252BE1Tiw7joU6HlQ%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.distrelec.ch/de/arduino-mkr-wan-1310-arduino-abx00029/p/30163021?q=Arduino+mkr+1310&amp;pos=1&amp;origPos=1&amp;origPageSize=50&amp;track=true</t>
+  </si>
+  <si>
+    <t>https://www.distrelec.ch/de/gsm-antenne-2g-3g-4g-fl-klebebefestigung-arduino-x000016/p/30101972?q=Arduino+antenne&amp;pos=1&amp;origPos=1&amp;origPageSize=50&amp;track=true</t>
+  </si>
+  <si>
+    <t>https://www.distrelec.ch/de/grove-pir-bewegungssensor-seeed-studio-101020020/p/30069806?q=grove+pir&amp;pos=3&amp;origPos=3&amp;origPageSize=50&amp;track=true</t>
+  </si>
+  <si>
+    <t>https://www.distrelec.ch/de/digitaler-temperatur-und-feuchtigkeitssensor-am2320-5v-adafruit-3721/p/30139175?track=true&amp;no-cache=true&amp;marketingPopup=false</t>
   </si>
 </sst>
 </file>
@@ -271,17 +274,10 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_-* #,##0.00\ [$CHF-100C]_-;\-* #,##0.00\ [$CHF-100C]_-;_-* &quot;-&quot;??\ [$CHF-100C]_-;_-@_-"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -317,21 +313,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="3">
-    <cellStyle name="Link" xfId="2" builtinId="8"/>
-    <cellStyle name="Schlecht" xfId="1" builtinId="27"/>
+  <cellStyles count="2">
+    <cellStyle name="Link" xfId="1" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -644,10 +637,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3693809-0733-4933-81AB-A7C1E8485E70}">
-  <dimension ref="A1:I27"/>
+  <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I31" sqref="I31"/>
+      <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -659,7 +652,7 @@
     <col min="5" max="5" width="30.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -676,10 +669,10 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -703,10 +696,10 @@
         <v>4.55</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -726,14 +719,14 @@
         <v>0.62</v>
       </c>
       <c r="G3" s="2">
-        <f t="shared" ref="G3:G25" si="0">F3*D3</f>
+        <f t="shared" ref="G3:G24" si="0">F3*D3</f>
         <v>0.62</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -749,41 +742,39 @@
       <c r="E4" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="2"/>
+      <c r="F4" s="2">
+        <v>47.17</v>
+      </c>
       <c r="G4" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>47.17</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="I4" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="D5">
         <v>1</v>
       </c>
-      <c r="F5" s="2"/>
+      <c r="F5" s="2">
+        <v>5.18</v>
+      </c>
       <c r="G5" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5.18</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="I5" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -807,13 +798,10 @@
         <v>0.17</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="I6" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -829,13 +817,18 @@
       <c r="E7" t="s">
         <v>18</v>
       </c>
-      <c r="F7" s="2"/>
+      <c r="F7" s="2">
+        <v>0.77</v>
+      </c>
       <c r="G7" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+        <v>0.77</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -859,10 +852,10 @@
         <v>1.06</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -878,43 +871,53 @@
       <c r="E9" t="s">
         <v>23</v>
       </c>
-      <c r="F9" s="2"/>
+      <c r="F9" s="2">
+        <v>0.77</v>
+      </c>
       <c r="G9" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+        <v>0.77</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C10" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="D10">
         <v>1</v>
       </c>
       <c r="E10" t="s">
-        <v>25</v>
-      </c>
-      <c r="F10" s="2"/>
+        <v>26</v>
+      </c>
+      <c r="F10" s="2">
+        <v>0.21299999999999999</v>
+      </c>
       <c r="G10" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+        <v>0.21299999999999999</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C11" t="s">
-        <v>27</v>
+        <v>6</v>
       </c>
       <c r="D11">
         <v>1</v>
@@ -922,13 +925,18 @@
       <c r="E11" t="s">
         <v>28</v>
       </c>
-      <c r="F11" s="2"/>
+      <c r="F11" s="2">
+        <v>0.13</v>
+      </c>
       <c r="G11" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+        <v>0.13</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -936,131 +944,131 @@
         <v>29</v>
       </c>
       <c r="C12" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="D12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E12" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F12" s="2">
-        <v>0.21299999999999999</v>
+        <v>0.121</v>
       </c>
       <c r="G12" s="2">
         <f t="shared" si="0"/>
-        <v>0.21299999999999999</v>
+        <v>0.24199999999999999</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C13" t="s">
-        <v>6</v>
+        <v>33</v>
       </c>
       <c r="D13">
         <v>1</v>
       </c>
       <c r="E13" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F13" s="2">
-        <v>0.13</v>
+        <v>10.7</v>
       </c>
       <c r="G13" s="2">
         <f t="shared" si="0"/>
-        <v>0.13</v>
+        <v>10.7</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C14" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E14" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="F14" s="2">
-        <v>0.121</v>
+        <v>0.68</v>
       </c>
       <c r="G14" s="2">
         <f t="shared" si="0"/>
-        <v>0.24199999999999999</v>
+        <v>0.68</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C15" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D15">
         <v>1</v>
       </c>
       <c r="E15" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F15" s="2">
-        <v>10.7</v>
+        <v>1.35</v>
       </c>
       <c r="G15" s="2">
         <f t="shared" si="0"/>
-        <v>10.7</v>
+        <v>1.35</v>
       </c>
       <c r="H15" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C16" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="D16">
         <v>1</v>
       </c>
       <c r="E16" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="F16" s="2">
-        <v>0.68</v>
+        <v>5.83</v>
       </c>
       <c r="G16" s="2">
         <f t="shared" si="0"/>
-        <v>0.68</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>70</v>
+        <v>5.83</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
@@ -1068,84 +1076,71 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>42</v>
+        <v>13</v>
       </c>
       <c r="C17" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D17">
         <v>1</v>
       </c>
       <c r="E17" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="F17" s="2">
-        <v>1.35</v>
+        <v>0.38100000000000001</v>
       </c>
       <c r="G17" s="2">
         <f t="shared" si="0"/>
-        <v>1.35</v>
+        <v>0.38100000000000001</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
-      <c r="B18" t="s">
-        <v>46</v>
-      </c>
       <c r="C18" t="s">
-        <v>47</v>
+        <v>70</v>
       </c>
       <c r="D18">
-        <v>1</v>
-      </c>
-      <c r="E18" t="s">
-        <v>48</v>
+        <v>2</v>
       </c>
       <c r="F18" s="2">
-        <v>5.83</v>
+        <v>1.54</v>
       </c>
       <c r="G18" s="2">
         <f t="shared" si="0"/>
-        <v>5.83</v>
-      </c>
-      <c r="H18" s="4" t="s">
+        <v>3.08</v>
+      </c>
+      <c r="H18" s="1" t="s">
         <v>71</v>
-      </c>
-      <c r="I18" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
-      <c r="B19" t="s">
-        <v>13</v>
-      </c>
       <c r="C19" t="s">
+        <v>47</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="F19" s="2">
+        <v>18.63</v>
+      </c>
+      <c r="G19" s="2">
+        <f t="shared" si="0"/>
+        <v>18.63</v>
+      </c>
+      <c r="H19" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D19">
-        <v>1</v>
-      </c>
-      <c r="E19" t="s">
+      <c r="I19" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H19" t="s">
-        <v>45</v>
-      </c>
-      <c r="I19" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
@@ -1153,23 +1148,20 @@
         <v>19</v>
       </c>
       <c r="C20" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D20">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F20" s="2">
-        <v>18.63</v>
+        <v>0.54</v>
       </c>
       <c r="G20" s="2">
         <f t="shared" si="0"/>
-        <v>18.63</v>
+        <v>1.62</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="I20" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
@@ -1177,20 +1169,20 @@
         <v>20</v>
       </c>
       <c r="C21" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="D21">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F21" s="2">
-        <v>0.54</v>
+        <v>12.6</v>
       </c>
       <c r="G21" s="2">
         <f t="shared" si="0"/>
-        <v>1.62</v>
+        <v>12.6</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>56</v>
+        <v>75</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
@@ -1198,19 +1190,20 @@
         <v>21</v>
       </c>
       <c r="C22" t="s">
-        <v>63</v>
+        <v>24</v>
       </c>
       <c r="D22">
         <v>1</v>
       </c>
-      <c r="F22" s="2"/>
+      <c r="F22" s="2">
+        <v>4.5199999999999996</v>
+      </c>
       <c r="G22" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H22" s="1"/>
-      <c r="I22" t="s">
-        <v>73</v>
+        <v>4.5199999999999996</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
@@ -1218,19 +1211,21 @@
         <v>22</v>
       </c>
       <c r="C23" t="s">
-        <v>28</v>
+        <v>60</v>
       </c>
       <c r="D23">
         <v>1</v>
       </c>
-      <c r="F23" s="2"/>
+      <c r="F23">
+        <f>23.9/5</f>
+        <v>4.7799999999999994</v>
+      </c>
       <c r="G23" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H23" s="1"/>
+        <v>4.7799999999999994</v>
+      </c>
       <c r="I23" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
@@ -1238,58 +1233,52 @@
         <v>23</v>
       </c>
       <c r="C24" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D24">
         <v>1</v>
       </c>
+      <c r="F24">
+        <f>24.4/5</f>
+        <v>4.88</v>
+      </c>
       <c r="G24" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4.88</v>
       </c>
       <c r="I24" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A25">
-        <v>24</v>
-      </c>
-      <c r="C25" t="s">
-        <v>66</v>
-      </c>
-      <c r="D25">
-        <v>1</v>
-      </c>
-      <c r="G25" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I25" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="G27" s="2">
-        <f>SUM(G2:G26)</f>
-        <v>45.794999999999995</v>
+        <v>68</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G26" s="2">
+        <f>SUM(G2:G25)</f>
+        <v>129.92600000000002</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H20" r:id="rId1" xr:uid="{C508F70E-FA28-4368-BF01-59057B8CD570}"/>
+    <hyperlink ref="H19" r:id="rId1" xr:uid="{C508F70E-FA28-4368-BF01-59057B8CD570}"/>
     <hyperlink ref="H8" r:id="rId2" xr:uid="{E1A74617-9304-456E-ACA6-D4C94536904D}"/>
-    <hyperlink ref="H21" r:id="rId3" xr:uid="{1EFDFB7E-29DA-429F-A655-98C80B609C0E}"/>
+    <hyperlink ref="H20" r:id="rId3" xr:uid="{1EFDFB7E-29DA-429F-A655-98C80B609C0E}"/>
     <hyperlink ref="H2" r:id="rId4" xr:uid="{3DF6B9EF-5A3C-48B8-AEE3-CE784F08870B}"/>
-    <hyperlink ref="H12" r:id="rId5" xr:uid="{D48968ED-F4F0-4D0D-A2F9-B8BDBA439F35}"/>
-    <hyperlink ref="H13" r:id="rId6" xr:uid="{FE737C2A-132D-4C9F-B22D-93A9CDC91061}"/>
+    <hyperlink ref="H10" r:id="rId5" xr:uid="{D48968ED-F4F0-4D0D-A2F9-B8BDBA439F35}"/>
+    <hyperlink ref="H11" r:id="rId6" xr:uid="{FE737C2A-132D-4C9F-B22D-93A9CDC91061}"/>
     <hyperlink ref="H3" r:id="rId7" xr:uid="{F4357A9D-D7C7-4EA3-9597-3309D5773E69}"/>
-    <hyperlink ref="I20" r:id="rId8" xr:uid="{9C8DD180-3DD5-412A-B202-870C25CB3B7F}"/>
-    <hyperlink ref="H14" r:id="rId9" xr:uid="{441B9AA9-4012-45D8-8EC7-0C684F9DA13D}"/>
-    <hyperlink ref="H17" r:id="rId10" xr:uid="{6291E4F9-606B-4018-93C0-2C984788A1D7}"/>
-    <hyperlink ref="H16" r:id="rId11" xr:uid="{51221FF9-0FE0-40D9-94DE-5EB7B49480EA}"/>
-    <hyperlink ref="H18" r:id="rId12" xr:uid="{177C1112-A34C-49E3-AE2A-E7AF10A703E0}"/>
+    <hyperlink ref="I19" r:id="rId8" xr:uid="{9C8DD180-3DD5-412A-B202-870C25CB3B7F}"/>
+    <hyperlink ref="H12" r:id="rId9" xr:uid="{441B9AA9-4012-45D8-8EC7-0C684F9DA13D}"/>
+    <hyperlink ref="H15" r:id="rId10" xr:uid="{6291E4F9-606B-4018-93C0-2C984788A1D7}"/>
+    <hyperlink ref="H14" r:id="rId11" xr:uid="{51221FF9-0FE0-40D9-94DE-5EB7B49480EA}"/>
+    <hyperlink ref="H16" r:id="rId12" xr:uid="{177C1112-A34C-49E3-AE2A-E7AF10A703E0}"/>
     <hyperlink ref="H6" r:id="rId13" xr:uid="{05129F61-5A64-4272-A8DA-5138EEBD2A12}"/>
+    <hyperlink ref="H7" r:id="rId14" xr:uid="{F055F013-85D9-4AFA-95DD-AA9517F569CB}"/>
+    <hyperlink ref="H9" r:id="rId15" xr:uid="{9343B6B8-12A6-4016-90D3-7B65E691131C}"/>
+    <hyperlink ref="H18" r:id="rId16" xr:uid="{6DCD60C6-8C2E-430D-944E-3984562F8F32}"/>
+    <hyperlink ref="H17" r:id="rId17" xr:uid="{E8803679-950B-4478-B7C8-95D2FA791FD5}"/>
+    <hyperlink ref="H4" r:id="rId18" xr:uid="{A9DE178D-00FC-43D5-A091-60B1B752CE75}"/>
+    <hyperlink ref="H5" r:id="rId19" xr:uid="{B7427711-C6DF-49FB-88B8-5ED24B593635}"/>
+    <hyperlink ref="H21" r:id="rId20" xr:uid="{F5207D95-A0E2-499E-A94F-CD8C2BA7761B}"/>
+    <hyperlink ref="H22" r:id="rId21" xr:uid="{226963D1-88DC-4FDF-9464-746014EA1DB4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
PDFs of schematics created
</commit_message>
<xml_diff>
--- a/hardware/PCB/BOM_v0.1_r1.xlsx
+++ b/hardware/PCB/BOM_v0.1_r1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meier\Documents\Repos\lora\hardware\PCB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58D480D3-5B87-478B-87A9-539D5A529EE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AD2D7D3-FB45-488A-889F-2251DC0434EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16332" yWindow="720" windowWidth="25644" windowHeight="15960" xr2:uid="{BC3F5926-5C61-49F0-80BB-A13677373133}"/>
+    <workbookView xWindow="53088" yWindow="336" windowWidth="25644" windowHeight="15960" xr2:uid="{BC3F5926-5C61-49F0-80BB-A13677373133}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="81">
   <si>
     <t>Id</t>
   </si>
@@ -159,9 +159,6 @@
     <t>10uF</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>B1</t>
   </si>
   <si>
@@ -265,6 +262,21 @@
   </si>
   <si>
     <t>https://www.distrelec.ch/de/digitaler-temperatur-und-feuchtigkeitssensor-am2320-5v-adafruit-3721/p/30139175?track=true&amp;no-cache=true&amp;marketingPopup=false</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/1554D2GYSL/HM3459-ND/2359931?itemSeq=385358295</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/analog-devices-inc-maxim-integrated/DS3231SN/1197576?s=N4IgTCBcDaICIGUDMYkEYEDkDEBaTcIAugL5A</t>
+  </si>
+  <si>
+    <t>Link 1</t>
+  </si>
+  <si>
+    <t>Link 2</t>
+  </si>
+  <si>
+    <t>Link 3</t>
   </si>
 </sst>
 </file>
@@ -637,10 +649,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3693809-0733-4933-81AB-A7C1E8485E70}">
-  <dimension ref="A1:I26"/>
+  <dimension ref="A1:J26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J28" sqref="J28"/>
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -652,7 +664,7 @@
     <col min="5" max="5" width="30.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -669,10 +681,19 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+      <c r="H1" t="s">
+        <v>78</v>
+      </c>
+      <c r="I1" t="s">
+        <v>79</v>
+      </c>
+      <c r="J1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -696,10 +717,10 @@
         <v>4.55</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -723,10 +744,10 @@
         <v>0.62</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -750,15 +771,15 @@
         <v>47.17</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -771,10 +792,10 @@
         <v>5.18</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -798,10 +819,10 @@
         <v>0.17</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -825,10 +846,10 @@
         <v>0.77</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -852,10 +873,10 @@
         <v>1.06</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -879,10 +900,10 @@
         <v>0.77</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -906,10 +927,10 @@
         <v>0.21299999999999999</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -933,10 +954,10 @@
         <v>0.13</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -960,10 +981,10 @@
         <v>0.24199999999999999</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -987,10 +1008,13 @@
         <v>10.7</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+        <v>58</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1014,10 +1038,10 @@
         <v>0.68</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1041,24 +1065,24 @@
         <v>1.35</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16" t="s">
         <v>42</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16" t="s">
         <v>43</v>
-      </c>
-      <c r="D16">
-        <v>1</v>
-      </c>
-      <c r="E16" t="s">
-        <v>44</v>
       </c>
       <c r="F16" s="2">
         <v>5.83</v>
@@ -1068,10 +1092,10 @@
         <v>5.83</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1079,13 +1103,13 @@
         <v>13</v>
       </c>
       <c r="C17" t="s">
+        <v>44</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17" t="s">
         <v>45</v>
-      </c>
-      <c r="D17">
-        <v>1</v>
-      </c>
-      <c r="E17" t="s">
-        <v>46</v>
       </c>
       <c r="F17" s="2">
         <v>0.38100000000000001</v>
@@ -1095,15 +1119,15 @@
         <v>0.38100000000000001</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="C18" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D18">
         <v>2</v>
@@ -1116,15 +1140,15 @@
         <v>3.08</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="C19" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D19">
         <v>1</v>
@@ -1137,18 +1161,21 @@
         <v>18.63</v>
       </c>
       <c r="H19" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="I19" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="I19" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J19" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="C20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D20">
         <v>3</v>
@@ -1161,15 +1188,15 @@
         <v>1.62</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="C21" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D21">
         <v>1</v>
@@ -1182,10 +1209,10 @@
         <v>12.6</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1203,15 +1230,15 @@
         <v>4.5199999999999996</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="C23" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D23">
         <v>1</v>
@@ -1225,15 +1252,15 @@
         <v>4.7799999999999994</v>
       </c>
       <c r="I23" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="C24" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D24">
         <v>1</v>
@@ -1247,10 +1274,10 @@
         <v>4.88</v>
       </c>
       <c r="I24" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="G26" s="2">
         <f>SUM(G2:G25)</f>
         <v>129.92600000000002</v>
@@ -1279,6 +1306,8 @@
     <hyperlink ref="H5" r:id="rId19" xr:uid="{B7427711-C6DF-49FB-88B8-5ED24B593635}"/>
     <hyperlink ref="H21" r:id="rId20" xr:uid="{F5207D95-A0E2-499E-A94F-CD8C2BA7761B}"/>
     <hyperlink ref="H22" r:id="rId21" xr:uid="{226963D1-88DC-4FDF-9464-746014EA1DB4}"/>
+    <hyperlink ref="J19" r:id="rId22" xr:uid="{4F14AA5E-CC66-4BEA-81A7-207DE79986BE}"/>
+    <hyperlink ref="I13" r:id="rId23" xr:uid="{2CC2CDE1-920D-47DF-BCF4-F69DAC74F275}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
payload formatter and BOM updated
</commit_message>
<xml_diff>
--- a/hardware/PCB/BOM_v0.1_r1.xlsx
+++ b/hardware/PCB/BOM_v0.1_r1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meier\Documents\Repos\lora\hardware\PCB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AD2D7D3-FB45-488A-889F-2251DC0434EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11272008-12AE-4EFC-B87F-B6A14CE1D4E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="53088" yWindow="336" windowWidth="25644" windowHeight="15960" xr2:uid="{BC3F5926-5C61-49F0-80BB-A13677373133}"/>
+    <workbookView xWindow="13788" yWindow="720" windowWidth="25644" windowHeight="15960" xr2:uid="{BC3F5926-5C61-49F0-80BB-A13677373133}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="83">
   <si>
     <t>Id</t>
   </si>
@@ -189,18 +189,12 @@
     <t>https://www.mouser.ch/ProductDetail/TE-Connectivity-Alcoswitch/MHS12204?qs=x%2FgbKjZ2T%2FPUluB%2FWhqq0Q%3D%3D</t>
   </si>
   <si>
-    <t>https://www.mouser.ch/ProductDetail/Wurth-Elektronik/971170321?qs=wr8lucFkNMVdX71b7R8Etg%3D%3D</t>
-  </si>
-  <si>
     <t>https://www.mouser.ch/ProductDetail/Bourns/CHP1206AFX-1002ELF?qs=sGAEpiMZZMtlubZbdhIBIA7Yl3UlZog1dCJD6gvx8dE%3D</t>
   </si>
   <si>
     <t>https://www.mouser.ch/ProductDetail/YAGEO/RT1206FRE071M2L?qs=sGAEpiMZZMtlubZbdhIBIBJfqA%2F7NWFP3T0Hpg54RHY%3D</t>
   </si>
   <si>
-    <t>https://www.mouser.ch/ProductDetail/YAGEO/RT1206FRE07330RL?qs=sGAEpiMZZMtlubZbdhIBIIe0KCL5sPzhE2j83oVm%252Bew%3D</t>
-  </si>
-  <si>
     <t>https://www.mouser.ch/ProductDetail/Keystone-Electronics/3000?qs=sGAEpiMZZMvxX9Q80wbhCYuFHF%2FXyzv7</t>
   </si>
   <si>
@@ -249,9 +243,6 @@
     <t>https://www.mouser.ch/ProductDetail/Harwin/M20-7821446?qs=Jph8NoUxIfX%2FjYzLF0Toqw%3D%3D</t>
   </si>
   <si>
-    <t>https://www.mouser.ch/ProductDetail/Samtec/TSW-102-17-L-S?qs=rU5fayqh%252BE1Tiw7joU6HlQ%3D%3D</t>
-  </si>
-  <si>
     <t>https://www.distrelec.ch/de/arduino-mkr-wan-1310-arduino-abx00029/p/30163021?q=Arduino+mkr+1310&amp;pos=1&amp;origPos=1&amp;origPageSize=50&amp;track=true</t>
   </si>
   <si>
@@ -277,6 +268,21 @@
   </si>
   <si>
     <t>Link 3</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ch/ProductDetail/Susumu/RG3216P-3303-D-T5?qs=nCAm%252BcMdy9yoDulF%2FHMGvA%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ch/ProductDetail/Wurth-Elektronik/971220321?qs=wr8lucFkNMXKaoSdjnz3%252Bg%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ch/ProductDetail/Samtec/TSW-102-19-L-S?qs=rU5fayqh%252BE00YQR0mRO7Kw%3D%3D</t>
+  </si>
+  <si>
+    <t>USB Kabel</t>
+  </si>
+  <si>
+    <t>https://www.reichelt.com/ch/de/usb-2-0-kabel-a-stecker-auf-90-micro-b-stecker-1-8-m-goobay-95343-p286822.html?PROVID=2808&amp;gclid=EAIaIQobChMI_PjA1-n-9AIVjLd3Ch0rvQDbEAQYAiABEgJUHfD_BwE</t>
   </si>
 </sst>
 </file>
@@ -649,10 +655,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3693809-0733-4933-81AB-A7C1E8485E70}">
-  <dimension ref="A1:J26"/>
+  <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+      <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -681,16 +687,16 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="H1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="I1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="J1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
@@ -717,7 +723,7 @@
         <v>4.55</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
@@ -740,11 +746,11 @@
         <v>0.62</v>
       </c>
       <c r="G3" s="2">
-        <f t="shared" ref="G3:G24" si="0">F3*D3</f>
+        <f t="shared" ref="G3:G25" si="0">F3*D3</f>
         <v>0.62</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
@@ -771,7 +777,7 @@
         <v>47.17</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
@@ -779,7 +785,7 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -792,7 +798,7 @@
         <v>5.18</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
@@ -819,7 +825,7 @@
         <v>0.17</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
@@ -846,7 +852,7 @@
         <v>0.77</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
@@ -900,7 +906,7 @@
         <v>0.77</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
@@ -927,7 +933,7 @@
         <v>0.21299999999999999</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
@@ -954,7 +960,7 @@
         <v>0.13</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>54</v>
+        <v>78</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
@@ -981,7 +987,7 @@
         <v>0.24199999999999999</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
@@ -1008,10 +1014,10 @@
         <v>10.7</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
@@ -1038,7 +1044,7 @@
         <v>0.68</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
@@ -1065,7 +1071,7 @@
         <v>1.35</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
@@ -1092,7 +1098,7 @@
         <v>5.83</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
@@ -1119,7 +1125,7 @@
         <v>0.38100000000000001</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
@@ -1127,7 +1133,7 @@
         <v>17</v>
       </c>
       <c r="C18" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D18">
         <v>2</v>
@@ -1140,7 +1146,7 @@
         <v>3.08</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
@@ -1167,7 +1173,7 @@
         <v>49</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
@@ -1188,7 +1194,7 @@
         <v>1.62</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>51</v>
+        <v>79</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
@@ -1196,7 +1202,7 @@
         <v>20</v>
       </c>
       <c r="C21" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D21">
         <v>1</v>
@@ -1209,7 +1215,7 @@
         <v>12.6</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
@@ -1230,7 +1236,7 @@
         <v>4.5199999999999996</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
@@ -1238,7 +1244,7 @@
         <v>22</v>
       </c>
       <c r="C23" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D23">
         <v>1</v>
@@ -1252,7 +1258,7 @@
         <v>4.7799999999999994</v>
       </c>
       <c r="I23" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
@@ -1260,7 +1266,7 @@
         <v>23</v>
       </c>
       <c r="C24" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D24">
         <v>1</v>
@@ -1274,40 +1280,59 @@
         <v>4.88</v>
       </c>
       <c r="I24" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="G26" s="2">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="C25" t="s">
+        <v>81</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="F25" s="2">
+        <v>2.02</v>
+      </c>
+      <c r="G25" s="2">
+        <f t="shared" si="0"/>
+        <v>2.02</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G28" s="2">
         <f>SUM(G2:G25)</f>
-        <v>129.92600000000002</v>
+        <v>131.94600000000003</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="H19" r:id="rId1" xr:uid="{C508F70E-FA28-4368-BF01-59057B8CD570}"/>
     <hyperlink ref="H8" r:id="rId2" xr:uid="{E1A74617-9304-456E-ACA6-D4C94536904D}"/>
-    <hyperlink ref="H20" r:id="rId3" xr:uid="{1EFDFB7E-29DA-429F-A655-98C80B609C0E}"/>
-    <hyperlink ref="H2" r:id="rId4" xr:uid="{3DF6B9EF-5A3C-48B8-AEE3-CE784F08870B}"/>
-    <hyperlink ref="H10" r:id="rId5" xr:uid="{D48968ED-F4F0-4D0D-A2F9-B8BDBA439F35}"/>
-    <hyperlink ref="H11" r:id="rId6" xr:uid="{FE737C2A-132D-4C9F-B22D-93A9CDC91061}"/>
-    <hyperlink ref="H3" r:id="rId7" xr:uid="{F4357A9D-D7C7-4EA3-9597-3309D5773E69}"/>
-    <hyperlink ref="I19" r:id="rId8" xr:uid="{9C8DD180-3DD5-412A-B202-870C25CB3B7F}"/>
-    <hyperlink ref="H12" r:id="rId9" xr:uid="{441B9AA9-4012-45D8-8EC7-0C684F9DA13D}"/>
-    <hyperlink ref="H15" r:id="rId10" xr:uid="{6291E4F9-606B-4018-93C0-2C984788A1D7}"/>
-    <hyperlink ref="H14" r:id="rId11" xr:uid="{51221FF9-0FE0-40D9-94DE-5EB7B49480EA}"/>
-    <hyperlink ref="H16" r:id="rId12" xr:uid="{177C1112-A34C-49E3-AE2A-E7AF10A703E0}"/>
-    <hyperlink ref="H6" r:id="rId13" xr:uid="{05129F61-5A64-4272-A8DA-5138EEBD2A12}"/>
-    <hyperlink ref="H7" r:id="rId14" xr:uid="{F055F013-85D9-4AFA-95DD-AA9517F569CB}"/>
-    <hyperlink ref="H9" r:id="rId15" xr:uid="{9343B6B8-12A6-4016-90D3-7B65E691131C}"/>
-    <hyperlink ref="H18" r:id="rId16" xr:uid="{6DCD60C6-8C2E-430D-944E-3984562F8F32}"/>
-    <hyperlink ref="H17" r:id="rId17" xr:uid="{E8803679-950B-4478-B7C8-95D2FA791FD5}"/>
-    <hyperlink ref="H4" r:id="rId18" xr:uid="{A9DE178D-00FC-43D5-A091-60B1B752CE75}"/>
-    <hyperlink ref="H5" r:id="rId19" xr:uid="{B7427711-C6DF-49FB-88B8-5ED24B593635}"/>
-    <hyperlink ref="H21" r:id="rId20" xr:uid="{F5207D95-A0E2-499E-A94F-CD8C2BA7761B}"/>
-    <hyperlink ref="H22" r:id="rId21" xr:uid="{226963D1-88DC-4FDF-9464-746014EA1DB4}"/>
-    <hyperlink ref="J19" r:id="rId22" xr:uid="{4F14AA5E-CC66-4BEA-81A7-207DE79986BE}"/>
-    <hyperlink ref="I13" r:id="rId23" xr:uid="{2CC2CDE1-920D-47DF-BCF4-F69DAC74F275}"/>
+    <hyperlink ref="H2" r:id="rId3" xr:uid="{3DF6B9EF-5A3C-48B8-AEE3-CE784F08870B}"/>
+    <hyperlink ref="H10" r:id="rId4" xr:uid="{D48968ED-F4F0-4D0D-A2F9-B8BDBA439F35}"/>
+    <hyperlink ref="H3" r:id="rId5" xr:uid="{F4357A9D-D7C7-4EA3-9597-3309D5773E69}"/>
+    <hyperlink ref="I19" r:id="rId6" xr:uid="{9C8DD180-3DD5-412A-B202-870C25CB3B7F}"/>
+    <hyperlink ref="H12" r:id="rId7" xr:uid="{441B9AA9-4012-45D8-8EC7-0C684F9DA13D}"/>
+    <hyperlink ref="H15" r:id="rId8" xr:uid="{6291E4F9-606B-4018-93C0-2C984788A1D7}"/>
+    <hyperlink ref="H14" r:id="rId9" xr:uid="{51221FF9-0FE0-40D9-94DE-5EB7B49480EA}"/>
+    <hyperlink ref="H16" r:id="rId10" xr:uid="{177C1112-A34C-49E3-AE2A-E7AF10A703E0}"/>
+    <hyperlink ref="H6" r:id="rId11" xr:uid="{05129F61-5A64-4272-A8DA-5138EEBD2A12}"/>
+    <hyperlink ref="H7" r:id="rId12" xr:uid="{F055F013-85D9-4AFA-95DD-AA9517F569CB}"/>
+    <hyperlink ref="H9" r:id="rId13" xr:uid="{9343B6B8-12A6-4016-90D3-7B65E691131C}"/>
+    <hyperlink ref="H18" r:id="rId14" xr:uid="{6DCD60C6-8C2E-430D-944E-3984562F8F32}"/>
+    <hyperlink ref="H4" r:id="rId15" xr:uid="{A9DE178D-00FC-43D5-A091-60B1B752CE75}"/>
+    <hyperlink ref="H5" r:id="rId16" xr:uid="{B7427711-C6DF-49FB-88B8-5ED24B593635}"/>
+    <hyperlink ref="H21" r:id="rId17" xr:uid="{F5207D95-A0E2-499E-A94F-CD8C2BA7761B}"/>
+    <hyperlink ref="H22" r:id="rId18" xr:uid="{226963D1-88DC-4FDF-9464-746014EA1DB4}"/>
+    <hyperlink ref="J19" r:id="rId19" xr:uid="{4F14AA5E-CC66-4BEA-81A7-207DE79986BE}"/>
+    <hyperlink ref="I13" r:id="rId20" xr:uid="{2CC2CDE1-920D-47DF-BCF4-F69DAC74F275}"/>
+    <hyperlink ref="H25" r:id="rId21" xr:uid="{DAC19965-3248-4E17-80BF-16BAE5E7C2FE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
timerSchedule unit tests finished
</commit_message>
<xml_diff>
--- a/hardware/PCB/BOM_v0.1_r1.xlsx
+++ b/hardware/PCB/BOM_v0.1_r1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meier\Documents\repos\lora\hardware\PCB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE5B3DD9-80E4-4B2A-8862-D60618C23FDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A23C129A-1548-4285-B566-B9835EA92A48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1152" yWindow="1152" windowWidth="30960" windowHeight="12264" xr2:uid="{BC3F5926-5C61-49F0-80BB-A13677373133}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16896" xr2:uid="{BC3F5926-5C61-49F0-80BB-A13677373133}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="86">
   <si>
     <t>Id</t>
   </si>
@@ -286,6 +286,12 @@
   </si>
   <si>
     <t>https://www.mouser.ch/ProductDetail/Murata-Electronics/GCJ31CD7YA106KE02L?qs=DPoM0jnrROWHhAptP6iQ0Q%3D%3D</t>
+  </si>
+  <si>
+    <t>Akku</t>
+  </si>
+  <si>
+    <t>https://www.conrad.ch/de/p/samsung-inr18650-29e-spezial-akku-18650-flat-top-hochtemperaturfaehig-li-ion-3-6-v-2900-mah-2239492.html?searchType=SearchRedirect</t>
   </si>
 </sst>
 </file>
@@ -674,10 +680,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3693809-0733-4933-81AB-A7C1E8485E70}">
-  <dimension ref="A1:J28"/>
+  <dimension ref="A1:J29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -765,7 +771,7 @@
         <v>0.62</v>
       </c>
       <c r="G3" s="2">
-        <f t="shared" ref="G3:G25" si="0">F3*D3</f>
+        <f t="shared" ref="G3:G26" si="0">F3*D3</f>
         <v>0.62</v>
       </c>
       <c r="H3" s="1" t="s">
@@ -1326,10 +1332,31 @@
         <v>82</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="G28" s="2">
-        <f>SUM(G2:G25)</f>
-        <v>131.94600000000003</v>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="C26" t="s">
+        <v>84</v>
+      </c>
+      <c r="D26">
+        <v>2</v>
+      </c>
+      <c r="F26" s="2">
+        <v>12.95</v>
+      </c>
+      <c r="G26" s="2">
+        <f t="shared" si="0"/>
+        <v>25.9</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G29" s="2">
+        <f>SUM(G2:G26)</f>
+        <v>157.84600000000003</v>
       </c>
     </row>
   </sheetData>
@@ -1358,6 +1385,7 @@
     <hyperlink ref="H11" r:id="rId22" xr:uid="{C10D9C33-FA68-4D6D-915A-2B8455A00DA2}"/>
     <hyperlink ref="H17" r:id="rId23" xr:uid="{3585FCDF-6DED-4540-8CD0-0C3F6737612F}"/>
     <hyperlink ref="H20" r:id="rId24" xr:uid="{DD24A338-F5ED-4EC8-B193-2562855F2A8E}"/>
+    <hyperlink ref="H26" r:id="rId25" xr:uid="{23982FC5-67B2-41B4-8AE6-EAC28C1E2DD0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>